<commit_message>
mon oct 25 make sure pre and most same length
</commit_message>
<xml_diff>
--- a/2014-2020_by_gender_by_year.xlsx
+++ b/2014-2020_by_gender_by_year.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>YEAR</t>
   </si>
   <si>
-    <t>Total num</t>
-  </si>
-  <si>
     <t>Pre Score F</t>
   </si>
   <si>
@@ -110,12 +107,6 @@
   </si>
   <si>
     <t>2018 112</t>
-  </si>
-  <si>
-    <t>2020 111</t>
-  </si>
-  <si>
-    <t>2020 112</t>
   </si>
 </sst>
 </file>
@@ -473,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,848 +534,673 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>122</v>
+        <v>12.22222222222222</v>
       </c>
       <c r="D2">
-        <v>12.29411764705882</v>
+        <v>0.8299256927239462</v>
       </c>
       <c r="E2">
-        <v>0.7747455585593874</v>
+        <v>16.26666666666667</v>
       </c>
       <c r="F2">
-        <v>16.26666666666667</v>
+        <v>0.961585391240146</v>
       </c>
       <c r="G2">
-        <v>0.961585391240146</v>
+        <v>4.044444444444444</v>
       </c>
       <c r="H2">
-        <v>3.972549019607841</v>
+        <v>0.2275</v>
       </c>
       <c r="I2">
-        <v>0.2243632336655592</v>
+        <v>0.02844124330170442</v>
       </c>
       <c r="J2">
-        <v>0.02844124330170442</v>
+        <v>1.270205936094532</v>
       </c>
       <c r="K2">
-        <v>1.234859160047801</v>
+        <v>0.4840439452830782</v>
       </c>
       <c r="L2">
-        <v>0.4840439452830782</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>51</v>
+        <v>18.98387096774194</v>
       </c>
       <c r="N2">
-        <v>19.04225352112676</v>
+        <v>0.7222723760724706</v>
       </c>
       <c r="O2">
-        <v>0.7144489285571241</v>
+        <v>20.46774193548387</v>
       </c>
       <c r="P2">
-        <v>20.46774193548387</v>
+        <v>0.7991659262316229</v>
       </c>
       <c r="Q2">
-        <v>0.7991659262316229</v>
+        <v>1.483870967741936</v>
       </c>
       <c r="R2">
-        <v>1.425488414357112</v>
+        <v>0.1346998535871157</v>
       </c>
       <c r="S2">
-        <v>0.1300895596649806</v>
+        <v>0.05000719128523947</v>
       </c>
       <c r="T2">
-        <v>0.05000719128523947</v>
+        <v>1.077192444685266</v>
       </c>
       <c r="U2">
-        <v>1.071962428989967</v>
+        <v>0.4385821197580691</v>
       </c>
       <c r="V2">
-        <v>0.4385821197580691</v>
-      </c>
-      <c r="W2">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>187</v>
+        <v>8.31</v>
       </c>
       <c r="D3">
-        <v>8.441441441441441</v>
+        <v>0.3532518488088472</v>
       </c>
       <c r="E3">
-        <v>0.3387805574758054</v>
+        <v>11.18</v>
       </c>
       <c r="F3">
-        <v>11.18</v>
+        <v>0.4684770080491754</v>
       </c>
       <c r="G3">
-        <v>0.4684770080491754</v>
+        <v>2.869999999999999</v>
       </c>
       <c r="H3">
-        <v>2.738558558558559</v>
+        <v>0.132319041032734</v>
       </c>
       <c r="I3">
-        <v>0.1270288340994568</v>
+        <v>0.01742777995922866</v>
       </c>
       <c r="J3">
-        <v>0.01742777995922866</v>
+        <v>0.5867346723669702</v>
       </c>
       <c r="K3">
-        <v>0.5781375037085249</v>
+        <v>0.3608785575970583</v>
       </c>
       <c r="L3">
-        <v>0.3608785575970583</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>111</v>
+        <v>13.17741935483871</v>
       </c>
       <c r="N3">
-        <v>12.85526315789474</v>
+        <v>0.5910151318407346</v>
       </c>
       <c r="O3">
-        <v>0.5135715831376025</v>
+        <v>14.83870967741935</v>
       </c>
       <c r="P3">
-        <v>14.83870967741935</v>
+        <v>0.7352259096542473</v>
       </c>
       <c r="Q3">
-        <v>0.7352259096542473</v>
+        <v>1.661290322580644</v>
       </c>
       <c r="R3">
-        <v>1.983446519524618</v>
+        <v>0.09875359539789065</v>
       </c>
       <c r="S3">
-        <v>0.1156883618448741</v>
+        <v>0.04496989452239333</v>
       </c>
       <c r="T3">
-        <v>0.04496989452239333</v>
+        <v>0.9433218031465384</v>
       </c>
       <c r="U3">
-        <v>0.8968349397929247</v>
+        <v>0.6170259902574159</v>
       </c>
       <c r="V3">
-        <v>0.6170259902574159</v>
-      </c>
-      <c r="W3">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4">
-        <v>190</v>
+        <v>12.1625</v>
       </c>
       <c r="D4">
-        <v>12.17441860465116</v>
+        <v>0.5738068937071275</v>
       </c>
       <c r="E4">
-        <v>0.5488931432927485</v>
+        <v>14.1875</v>
       </c>
       <c r="F4">
-        <v>14.1875</v>
+        <v>0.5974878183176412</v>
       </c>
       <c r="G4">
-        <v>0.5974878183176412</v>
+        <v>2.025</v>
       </c>
       <c r="H4">
-        <v>2.013081395348838</v>
+        <v>0.1135248773651016</v>
       </c>
       <c r="I4">
-        <v>0.1129321591650359</v>
+        <v>0.02285394666213483</v>
       </c>
       <c r="J4">
-        <v>0.02285394666213483</v>
+        <v>0.8283996887395584</v>
       </c>
       <c r="K4">
-        <v>0.8113417133315458</v>
+        <v>0.3601928983900611</v>
       </c>
       <c r="L4">
-        <v>0.3601928983900611</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>86</v>
+        <v>17.15555555555556</v>
       </c>
       <c r="N4">
-        <v>17</v>
+        <v>0.6805503961688807</v>
       </c>
       <c r="O4">
-        <v>0.6225774558828503</v>
+        <v>19.6</v>
       </c>
       <c r="P4">
-        <v>19.6</v>
+        <v>0.7672770734003416</v>
       </c>
       <c r="Q4">
-        <v>0.7672770734003416</v>
+        <v>2.444444444444446</v>
       </c>
       <c r="R4">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="S4">
-        <v>0.2000000000000001</v>
+        <v>0.1903114186851212</v>
+      </c>
+      <c r="T4">
+        <v>1.025603699823384</v>
       </c>
       <c r="U4">
-        <v>0.9880874434681151</v>
+        <v>0.4189968136698011</v>
       </c>
       <c r="V4">
-        <v>0.4189968136698011</v>
-      </c>
-      <c r="W4">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>219</v>
+        <v>8.467213114754099</v>
       </c>
       <c r="D5">
-        <v>8.4765625</v>
+        <v>0.3570917062688789</v>
       </c>
       <c r="E5">
-        <v>0.3420506211511273</v>
+        <v>12.09016393442623</v>
       </c>
       <c r="F5">
-        <v>12.09016393442623</v>
+        <v>0.4473353793918954</v>
       </c>
       <c r="G5">
-        <v>0.4473353793918954</v>
+        <v>3.622950819672131</v>
       </c>
       <c r="H5">
-        <v>3.613601434426229</v>
+        <v>0.1682527598020556</v>
       </c>
       <c r="I5">
-        <v>0.1678914641040136</v>
+        <v>0.01657304314922326</v>
       </c>
       <c r="J5">
-        <v>0.01657304314922326</v>
+        <v>0.5723839867970716</v>
       </c>
       <c r="K5">
-        <v>0.563123049684137</v>
+        <v>0.3502235469448585</v>
       </c>
       <c r="L5">
-        <v>0.3502235469448585</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>128</v>
+        <v>12.98837209302326</v>
       </c>
       <c r="N5">
-        <v>13.02222222222222</v>
+        <v>0.5837503603309038</v>
       </c>
       <c r="O5">
-        <v>0.5766963854951237</v>
+        <v>16.66279069767442</v>
       </c>
       <c r="P5">
-        <v>16.52873563218391</v>
+        <v>0.688703149956194</v>
       </c>
       <c r="Q5">
-        <v>0.693814863305895</v>
+        <v>3.67441860465116</v>
       </c>
       <c r="R5">
-        <v>3.506513409961684</v>
+        <v>0.2159945317840054</v>
       </c>
       <c r="S5">
-        <v>0.2065354757176385</v>
+        <v>0.03037152493102834</v>
       </c>
       <c r="T5">
-        <v>0.03037152493102834</v>
+        <v>0.9028158793165103</v>
       </c>
       <c r="U5">
-        <v>0.9021960904300783</v>
+        <v>0.4424288949386546</v>
       </c>
       <c r="V5">
-        <v>0.4424288949386546</v>
-      </c>
-      <c r="W5">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:22">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>221</v>
+        <v>12.65909090909091</v>
       </c>
       <c r="D6">
-        <v>12.55913978494624</v>
+        <v>0.5532950512141868</v>
       </c>
       <c r="E6">
-        <v>0.5325897031142705</v>
+        <v>15.07954545454546</v>
       </c>
       <c r="F6">
-        <v>14.98876404494382</v>
+        <v>0.5989414187727352</v>
       </c>
       <c r="G6">
-        <v>0.5990915795093753</v>
+        <v>2.420454545454547</v>
       </c>
       <c r="H6">
-        <v>2.429624259997585</v>
+        <v>0.1395806028833552</v>
       </c>
       <c r="I6">
-        <v>0.139306446473351</v>
+        <v>0.03027141051974356</v>
       </c>
       <c r="J6">
-        <v>0.0299898079537526</v>
+        <v>0.8153933019222114</v>
       </c>
       <c r="K6">
-        <v>0.8015999703732435</v>
+        <v>0.4324004076867678</v>
       </c>
       <c r="L6">
-        <v>0.4292383501986853</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>93</v>
+        <v>18.42477876106195</v>
       </c>
       <c r="N6">
-        <v>18.248</v>
+        <v>0.5386170234948955</v>
       </c>
       <c r="O6">
-        <v>0.5176442918677127</v>
+        <v>19.35398230088495</v>
       </c>
       <c r="P6">
-        <v>19.35398230088495</v>
+        <v>0.6576545731672686</v>
       </c>
       <c r="Q6">
-        <v>0.6576545731672686</v>
+        <v>0.929203539823007</v>
       </c>
       <c r="R6">
-        <v>1.105982300884953</v>
-      </c>
-      <c r="S6">
-        <v>0.09411013452050319</v>
+        <v>0.080275229357798</v>
+      </c>
+      <c r="T6">
+        <v>0.8500693122365511</v>
       </c>
       <c r="U6">
-        <v>0.8369379609690601</v>
+        <v>0.3660093360776047</v>
       </c>
       <c r="V6">
-        <v>0.3660093360776047</v>
-      </c>
-      <c r="W6">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:22">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>262</v>
+        <v>8.38036809815951</v>
       </c>
       <c r="D7">
-        <v>8.394117647058824</v>
+        <v>0.337758469669902</v>
       </c>
       <c r="E7">
-        <v>0.3306268302147993</v>
+        <v>13.14110429447853</v>
       </c>
       <c r="F7">
-        <v>13.14110429447853</v>
+        <v>0.4233112369027712</v>
       </c>
       <c r="G7">
-        <v>0.4233112369027712</v>
+        <v>4.760736196319018</v>
       </c>
       <c r="H7">
-        <v>4.746986647419703</v>
+        <v>0.2202043132803632</v>
       </c>
       <c r="I7">
-        <v>0.2197080669919275</v>
+        <v>0.02606069692203975</v>
       </c>
       <c r="J7">
-        <v>0.02606069692203975</v>
+        <v>0.5415470313111393</v>
       </c>
       <c r="K7">
-        <v>0.5371280146725171</v>
+        <v>0.3619644739167225</v>
       </c>
       <c r="L7">
-        <v>0.3619644739167225</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>170</v>
+        <v>13.71604938271605</v>
       </c>
       <c r="N7">
-        <v>13.79120879120879</v>
+        <v>0.6216849287113214</v>
       </c>
       <c r="O7">
-        <v>0.585439209494712</v>
+        <v>17.59259259259259</v>
       </c>
       <c r="P7">
-        <v>17.48780487804878</v>
+        <v>0.7618969539576407</v>
       </c>
       <c r="Q7">
-        <v>0.7598086698811521</v>
+        <v>3.876543209876543</v>
       </c>
       <c r="R7">
-        <v>3.696596086839989</v>
+        <v>0.2380591357088704</v>
       </c>
       <c r="S7">
-        <v>0.2280611823067383</v>
+        <v>0.04300290687862524</v>
       </c>
       <c r="T7">
-        <v>0.04300290687862524</v>
+        <v>0.9833509643238939</v>
       </c>
       <c r="U7">
-        <v>0.9591914735027407</v>
+        <v>0.5481119996978467</v>
       </c>
       <c r="V7">
-        <v>0.5481119996978467</v>
-      </c>
-      <c r="W7">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8">
-        <v>175</v>
+        <v>13.46153846153846</v>
       </c>
       <c r="D8">
-        <v>13.54545454545454</v>
+        <v>0.8444037846192365</v>
       </c>
       <c r="E8">
-        <v>0.83919882500575</v>
+        <v>15.01923076923077</v>
       </c>
       <c r="F8">
-        <v>15.01923076923077</v>
+        <v>0.8832659062239271</v>
       </c>
       <c r="G8">
-        <v>0.8832659062239271</v>
+        <v>1.557692307692308</v>
       </c>
       <c r="H8">
-        <v>1.473776223776225</v>
+        <v>0.09418604651162794</v>
       </c>
       <c r="I8">
-        <v>0.08956651083722915</v>
+        <v>0.05372298577769118</v>
       </c>
       <c r="J8">
-        <v>0.05372298577769118</v>
+        <v>1.221955978166507</v>
       </c>
       <c r="K8">
-        <v>1.218365022884606</v>
+        <v>0.5391277391388291</v>
       </c>
       <c r="L8">
-        <v>0.5391277391388291</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>55</v>
+        <v>18.19090909090909</v>
       </c>
       <c r="N8">
-        <v>18.025</v>
+        <v>0.6482793617466404</v>
       </c>
       <c r="O8">
-        <v>0.6216746269043758</v>
+        <v>20.03636363636364</v>
       </c>
       <c r="P8">
-        <v>20.03636363636364</v>
+        <v>0.6712153060758306</v>
       </c>
       <c r="Q8">
-        <v>0.6712153060758306</v>
+        <v>1.845454545454544</v>
       </c>
       <c r="R8">
-        <v>2.011363636363637</v>
-      </c>
-      <c r="S8">
-        <v>0.1679635604479028</v>
+        <v>0.1562740569668975</v>
+      </c>
+      <c r="T8">
+        <v>0.9331645717541479</v>
       </c>
       <c r="U8">
-        <v>0.9148821393202328</v>
+        <v>0.4667754206794948</v>
       </c>
       <c r="V8">
-        <v>0.4667754206794948</v>
-      </c>
-      <c r="W8">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9">
-        <v>251</v>
+        <v>9.341935483870968</v>
       </c>
       <c r="D9">
-        <v>9.282208588957054</v>
+        <v>0.3613546534383871</v>
       </c>
       <c r="E9">
-        <v>0.3492571403148321</v>
+        <v>14.69677419354839</v>
       </c>
       <c r="F9">
-        <v>14.69677419354839</v>
+        <v>0.4553249799113191</v>
       </c>
       <c r="G9">
-        <v>0.4553249799113191</v>
+        <v>5.35483870967742</v>
       </c>
       <c r="H9">
-        <v>5.414565604591333</v>
+        <v>0.259212991880075</v>
       </c>
       <c r="I9">
-        <v>0.261348591515661</v>
+        <v>0.01840167632098874</v>
       </c>
       <c r="J9">
-        <v>0.01840167632098874</v>
+        <v>0.5812899645554016</v>
       </c>
       <c r="K9">
-        <v>0.5738478782675226</v>
+        <v>0.3698686839386575</v>
       </c>
       <c r="L9">
-        <v>0.3698686839386575</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>163</v>
+        <v>15.06410256410256</v>
       </c>
       <c r="N9">
-        <v>14.73255813953488</v>
+        <v>0.6585435204259115</v>
       </c>
       <c r="O9">
-        <v>0.6275534800662569</v>
+        <v>20.2948717948718</v>
       </c>
       <c r="P9">
-        <v>20.4</v>
+        <v>0.6093698875011779</v>
       </c>
       <c r="Q9">
-        <v>0.6002636551518028</v>
+        <v>5.230769230769232</v>
       </c>
       <c r="R9">
-        <v>5.667441860465114</v>
-      </c>
-      <c r="S9">
-        <v>0.3712109672505711</v>
+        <v>0.3502145922746782</v>
+      </c>
+      <c r="T9">
+        <v>0.897224179393395</v>
       </c>
       <c r="U9">
-        <v>0.8684122442938448</v>
+        <v>0.4913243592729864</v>
       </c>
       <c r="V9">
-        <v>0.4913243592729864</v>
-      </c>
-      <c r="W9">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
-        <v>159</v>
+        <v>11.97674418604651</v>
       </c>
       <c r="D10">
-        <v>11.95652173913044</v>
+        <v>0.8113865551343201</v>
       </c>
       <c r="E10">
-        <v>0.7906192288107742</v>
+        <v>12.81395348837209</v>
       </c>
       <c r="F10">
-        <v>12.81395348837209</v>
+        <v>0.9749099478267346</v>
       </c>
       <c r="G10">
-        <v>0.9749099478267346</v>
+        <v>0.8372093023255811</v>
       </c>
       <c r="H10">
-        <v>0.8574317492416572</v>
+        <v>0.04645161290322579</v>
       </c>
       <c r="I10">
-        <v>0.04752031381339306</v>
+        <v>0.03889853635251428</v>
       </c>
       <c r="J10">
-        <v>0.03889853635251428</v>
+        <v>1.268383833161029</v>
       </c>
       <c r="K10">
-        <v>1.255200450659921</v>
+        <v>0.690009575549571</v>
       </c>
       <c r="L10">
-        <v>0.690009575549571</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>46</v>
+        <v>17.36842105263158</v>
       </c>
       <c r="N10">
-        <v>17.05309734513274</v>
+        <v>0.6797424964615975</v>
       </c>
       <c r="O10">
-        <v>0.6324106433840717</v>
+        <v>17.2421052631579</v>
       </c>
       <c r="P10">
-        <v>17.2421052631579</v>
+        <v>0.687386890131191</v>
       </c>
       <c r="Q10">
-        <v>0.687386890131191</v>
+        <v>-0.1263157894736828</v>
       </c>
       <c r="R10">
-        <v>0.1890079180251512</v>
+        <v>-0.009999999999999891</v>
       </c>
       <c r="S10">
-        <v>0.01459869770119076</v>
+        <v>0.03449851527697276</v>
       </c>
       <c r="T10">
-        <v>0.03449851527697276</v>
+        <v>0.9667215722327059</v>
       </c>
       <c r="U10">
-        <v>0.9340470858525739</v>
+        <v>0.3179025977388099</v>
       </c>
       <c r="V10">
-        <v>0.3179025977388099</v>
-      </c>
-      <c r="W10">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>287</v>
+        <v>9.790419161676647</v>
       </c>
       <c r="D11">
-        <v>9.771276595744681</v>
+        <v>0.3659081535133401</v>
       </c>
       <c r="E11">
-        <v>0.3373599292407899</v>
+        <v>14.10778443113773</v>
       </c>
       <c r="F11">
-        <v>14.10778443113773</v>
+        <v>0.4384840137280439</v>
       </c>
       <c r="G11">
-        <v>0.4384840137280439</v>
+        <v>4.317365269461078</v>
       </c>
       <c r="H11">
-        <v>4.336507835393045</v>
+        <v>0.2136296296296296</v>
       </c>
       <c r="I11">
-        <v>0.2143737767693643</v>
+        <v>0.0168850133911933</v>
       </c>
       <c r="J11">
-        <v>0.0168850133911933</v>
+        <v>0.5711015733672929</v>
       </c>
       <c r="K11">
-        <v>0.5532449296219588</v>
+        <v>0.318613100477558</v>
       </c>
       <c r="L11">
-        <v>0.318613100477558</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>188</v>
+        <v>14.45977011494253</v>
       </c>
       <c r="N11">
-        <v>14.28282828282828</v>
+        <v>0.5754499413888345</v>
       </c>
       <c r="O11">
-        <v>0.549739992896476</v>
+        <v>18.70114942528735</v>
       </c>
       <c r="P11">
-        <v>18.70114942528735</v>
+        <v>0.6580805569134573</v>
       </c>
       <c r="Q11">
-        <v>0.6580805569134573</v>
+        <v>4.241379310344826</v>
       </c>
       <c r="R11">
-        <v>4.418321142459073</v>
+        <v>0.2729289940828401</v>
       </c>
       <c r="S11">
-        <v>0.2811142629199538</v>
+        <v>0.03362558601135256</v>
       </c>
       <c r="T11">
-        <v>0.03362558601135256</v>
+        <v>0.8741925728533383</v>
       </c>
       <c r="U11">
-        <v>0.8574870723091652</v>
+        <v>0.46731315739378</v>
       </c>
       <c r="V11">
-        <v>0.46731315739378</v>
-      </c>
-      <c r="W11">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>224</v>
-      </c>
-      <c r="D12">
-        <v>12.31884057971014</v>
-      </c>
-      <c r="E12">
-        <v>0.6627633236671218</v>
-      </c>
-      <c r="F12">
-        <v>14.89473684210526</v>
-      </c>
-      <c r="G12">
-        <v>0.8012694386798697</v>
-      </c>
-      <c r="H12">
-        <v>2.575896262395119</v>
-      </c>
-      <c r="I12">
-        <v>0.1456859361518551</v>
-      </c>
-      <c r="J12">
-        <v>0.02304780461542826</v>
-      </c>
-      <c r="K12">
-        <v>1.039849958677041</v>
-      </c>
-      <c r="L12">
-        <v>0.6914341384628476</v>
-      </c>
-      <c r="M12">
-        <v>69</v>
-      </c>
-      <c r="N12">
-        <v>14.6258064516129</v>
-      </c>
-      <c r="O12">
-        <v>0.4327548746012478</v>
-      </c>
-      <c r="P12">
-        <v>17.96396396396396</v>
-      </c>
-      <c r="Q12">
-        <v>0.6985333796916776</v>
-      </c>
-      <c r="R12">
-        <v>3.33815751235106</v>
-      </c>
-      <c r="S12">
-        <v>0.2171273245549367</v>
-      </c>
-      <c r="T12">
-        <v>0.01909700426514009</v>
-      </c>
-      <c r="U12">
-        <v>0.572910127954203</v>
-      </c>
-      <c r="V12">
-        <v>0.8217211595393045</v>
-      </c>
-      <c r="W12">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13">
-        <v>360</v>
-      </c>
-      <c r="D13">
-        <v>9.381147540983607</v>
-      </c>
-      <c r="E13">
-        <v>0.2654379097425579</v>
-      </c>
-      <c r="F13">
-        <v>13.64651162790698</v>
-      </c>
-      <c r="G13">
-        <v>0.3863891347290506</v>
-      </c>
-      <c r="H13">
-        <v>4.26536408692337</v>
-      </c>
-      <c r="I13">
-        <v>0.2068671908585375</v>
-      </c>
-      <c r="J13">
-        <v>0.0103739092627643</v>
-      </c>
-      <c r="K13">
-        <v>0.4687791029527263</v>
-      </c>
-      <c r="L13">
-        <v>0.3112172778829289</v>
-      </c>
-      <c r="M13">
-        <v>244</v>
-      </c>
-      <c r="N13">
-        <v>11.78448275862069</v>
-      </c>
-      <c r="O13">
-        <v>0.4749822113741239</v>
-      </c>
-      <c r="P13">
-        <v>15.75308641975309</v>
-      </c>
-      <c r="Q13">
-        <v>0.8201796822477849</v>
-      </c>
-      <c r="R13">
-        <v>3.968603661132397</v>
-      </c>
-      <c r="S13">
-        <v>0.2178693917138467</v>
-      </c>
-      <c r="T13">
-        <v>0.02474924627020214</v>
-      </c>
-      <c r="U13">
-        <v>0.7424773881060645</v>
-      </c>
-      <c r="V13">
-        <v>0.9477883794887604</v>
-      </c>
-      <c r="W13">
-        <v>116</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nov 1 add mean to pre test by question
</commit_message>
<xml_diff>
--- a/2014-2020_by_gender_by_year.xlsx
+++ b/2014-2020_by_gender_by_year.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>YEAR</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>2018 112</t>
+  </si>
+  <si>
+    <t>2020 111</t>
+  </si>
+  <si>
+    <t>2020 112</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,7 +576,7 @@
         <v>0.4840439452830782</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M2">
         <v>18.98387096774194</v>
@@ -638,7 +644,7 @@
         <v>0.3608785575970583</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M3">
         <v>13.17741935483871</v>
@@ -706,7 +712,7 @@
         <v>0.3601928983900611</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M4">
         <v>17.15555555555556</v>
@@ -771,7 +777,7 @@
         <v>0.3502235469448585</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="M5">
         <v>12.98837209302326</v>
@@ -839,7 +845,7 @@
         <v>0.4324004076867678</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="M6">
         <v>18.42477876106195</v>
@@ -904,7 +910,7 @@
         <v>0.3619644739167225</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="M7">
         <v>13.71604938271605</v>
@@ -972,7 +978,7 @@
         <v>0.5391277391388291</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="M8">
         <v>18.19090909090909</v>
@@ -1037,7 +1043,7 @@
         <v>0.3698686839386575</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="M9">
         <v>15.06410256410256</v>
@@ -1102,7 +1108,7 @@
         <v>0.690009575549571</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="M10">
         <v>17.36842105263158</v>
@@ -1170,7 +1176,7 @@
         <v>0.318613100477558</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="M11">
         <v>14.45977011494253</v>
@@ -1201,6 +1207,142 @@
       </c>
       <c r="V11">
         <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>12.33333333333333</v>
+      </c>
+      <c r="D12">
+        <v>0.7072544488881022</v>
+      </c>
+      <c r="E12">
+        <v>14.89473684210526</v>
+      </c>
+      <c r="F12">
+        <v>0.8012694386798697</v>
+      </c>
+      <c r="G12">
+        <v>2.56140350877193</v>
+      </c>
+      <c r="H12">
+        <v>0.1449851042701092</v>
+      </c>
+      <c r="I12">
+        <v>0.02304780461542826</v>
+      </c>
+      <c r="J12">
+        <v>0.6914341384628476</v>
+      </c>
+      <c r="K12">
+        <v>1.068757020484248</v>
+      </c>
+      <c r="L12">
+        <v>57</v>
+      </c>
+      <c r="M12">
+        <v>14.76576576576577</v>
+      </c>
+      <c r="N12">
+        <v>0.5200256647977225</v>
+      </c>
+      <c r="O12">
+        <v>17.96396396396396</v>
+      </c>
+      <c r="P12">
+        <v>0.6985333796916776</v>
+      </c>
+      <c r="Q12">
+        <v>3.198198198198197</v>
+      </c>
+      <c r="R12">
+        <v>0.2099349497338852</v>
+      </c>
+      <c r="S12">
+        <v>0.01909700426514009</v>
+      </c>
+      <c r="T12">
+        <v>0.572910127954203</v>
+      </c>
+      <c r="U12">
+        <v>0.8708476184682317</v>
+      </c>
+      <c r="V12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>9.376744186046512</v>
+      </c>
+      <c r="D13">
+        <v>0.2736919344088321</v>
+      </c>
+      <c r="E13">
+        <v>13.64651162790698</v>
+      </c>
+      <c r="F13">
+        <v>0.3863891347290506</v>
+      </c>
+      <c r="G13">
+        <v>4.269767441860465</v>
+      </c>
+      <c r="H13">
+        <v>0.2070365358592693</v>
+      </c>
+      <c r="I13">
+        <v>0.0103739092627643</v>
+      </c>
+      <c r="J13">
+        <v>0.3112172778829289</v>
+      </c>
+      <c r="K13">
+        <v>0.473501677290707</v>
+      </c>
+      <c r="L13">
+        <v>215</v>
+      </c>
+      <c r="M13">
+        <v>12.24691358024691</v>
+      </c>
+      <c r="N13">
+        <v>0.5413548573186054</v>
+      </c>
+      <c r="O13">
+        <v>15.75308641975309</v>
+      </c>
+      <c r="P13">
+        <v>0.8201796822477849</v>
+      </c>
+      <c r="Q13">
+        <v>3.506172839506174</v>
+      </c>
+      <c r="R13">
+        <v>0.1974965229485397</v>
+      </c>
+      <c r="S13">
+        <v>0.02474924627020214</v>
+      </c>
+      <c r="T13">
+        <v>0.7424773881060645</v>
+      </c>
+      <c r="U13">
+        <v>0.9827307834369111</v>
+      </c>
+      <c r="V13">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ad by qiestion threshold
</commit_message>
<xml_diff>
--- a/2014-2020_by_gender_by_year.xlsx
+++ b/2014-2020_by_gender_by_year.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayapatel/Documents/_/honours/Honours-FCI-data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B0080-CA04-AF42-939C-ACEAB20FE0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="440" windowWidth="24420" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>YEAR</t>
   </si>
   <si>
+    <t>Avg Grade</t>
+  </si>
+  <si>
     <t>Pre Score F</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t>Num F</t>
   </si>
   <si>
+    <t>Avg Grade F</t>
+  </si>
+  <si>
     <t>Pre Score M</t>
   </si>
   <si>
@@ -77,6 +89,9 @@
   </si>
   <si>
     <t>Num M</t>
+  </si>
+  <si>
+    <t>Avg M Grade</t>
   </si>
   <si>
     <t>2014 111</t>
@@ -118,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +197,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -228,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,9 +283,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,6 +335,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,14 +528,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,809 +624,926 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2">
+        <v>69.474509803921563</v>
+      </c>
+      <c r="D2">
         <v>12.22222222222222</v>
       </c>
-      <c r="D2">
-        <v>0.8299256927239462</v>
-      </c>
       <c r="E2">
-        <v>16.26666666666667</v>
+        <v>0.82992569272394623</v>
       </c>
       <c r="F2">
-        <v>0.961585391240146</v>
+        <v>16.266666666666669</v>
       </c>
       <c r="G2">
-        <v>4.044444444444444</v>
+        <v>0.96158539124014597</v>
       </c>
       <c r="H2">
-        <v>0.2275</v>
+        <v>4.0444444444444443</v>
       </c>
       <c r="I2">
-        <v>0.02844124330170442</v>
+        <v>0.22750000000000001</v>
       </c>
       <c r="J2">
-        <v>1.270205936094532</v>
+        <v>2.844124330170442E-2</v>
       </c>
       <c r="K2">
+        <v>1.2702059360945319</v>
+      </c>
+      <c r="L2">
         <v>0.4840439452830782</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>45</v>
       </c>
-      <c r="M2">
-        <v>18.98387096774194</v>
-      </c>
       <c r="N2">
-        <v>0.7222723760724706</v>
+        <v>70.627450980392155</v>
       </c>
       <c r="O2">
-        <v>20.46774193548387</v>
+        <v>18.983870967741939</v>
       </c>
       <c r="P2">
-        <v>0.7991659262316229</v>
+        <v>0.72227237607247063</v>
       </c>
       <c r="Q2">
-        <v>1.483870967741936</v>
+        <v>20.467741935483868</v>
       </c>
       <c r="R2">
+        <v>0.79916592623162286</v>
+      </c>
+      <c r="S2">
+        <v>1.4838709677419359</v>
+      </c>
+      <c r="T2">
         <v>0.1346998535871157</v>
       </c>
-      <c r="S2">
-        <v>0.05000719128523947</v>
-      </c>
-      <c r="T2">
-        <v>1.077192444685266</v>
-      </c>
       <c r="U2">
+        <v>5.000719128523947E-2</v>
+      </c>
+      <c r="V2">
+        <v>1.0771924446852661</v>
+      </c>
+      <c r="W2">
         <v>0.4385821197580691</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>62</v>
       </c>
+      <c r="Y2">
+        <v>69.521126760563376</v>
+      </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C3">
+        <v>68.779527559055111</v>
+      </c>
+      <c r="D3">
         <v>8.31</v>
       </c>
-      <c r="D3">
-        <v>0.3532518488088472</v>
-      </c>
       <c r="E3">
+        <v>0.35325184880884719</v>
+      </c>
+      <c r="F3">
         <v>11.18</v>
       </c>
-      <c r="F3">
-        <v>0.4684770080491754</v>
-      </c>
       <c r="G3">
-        <v>2.869999999999999</v>
+        <v>0.46847700804917541</v>
       </c>
       <c r="H3">
-        <v>0.132319041032734</v>
+        <v>2.8699999999999992</v>
       </c>
       <c r="I3">
-        <v>0.01742777995922866</v>
+        <v>0.13231904103273401</v>
       </c>
       <c r="J3">
-        <v>0.5867346723669702</v>
+        <v>1.7427779959228659E-2</v>
       </c>
       <c r="K3">
-        <v>0.3608785575970583</v>
+        <v>0.58673467236697019</v>
       </c>
       <c r="L3">
+        <v>0.36087855759705828</v>
+      </c>
+      <c r="M3">
         <v>100</v>
       </c>
-      <c r="M3">
+      <c r="N3">
+        <v>71.414414414414409</v>
+      </c>
+      <c r="O3">
         <v>13.17741935483871</v>
       </c>
-      <c r="N3">
-        <v>0.5910151318407346</v>
-      </c>
-      <c r="O3">
-        <v>14.83870967741935</v>
-      </c>
       <c r="P3">
-        <v>0.7352259096542473</v>
+        <v>0.59101513184073462</v>
       </c>
       <c r="Q3">
-        <v>1.661290322580644</v>
+        <v>14.838709677419351</v>
       </c>
       <c r="R3">
-        <v>0.09875359539789065</v>
+        <v>0.73522590965424728</v>
       </c>
       <c r="S3">
-        <v>0.04496989452239333</v>
+        <v>1.6612903225806439</v>
       </c>
       <c r="T3">
-        <v>0.9433218031465384</v>
+        <v>9.8753595397890651E-2</v>
       </c>
       <c r="U3">
-        <v>0.6170259902574159</v>
+        <v>4.4969894522393333E-2</v>
       </c>
       <c r="V3">
+        <v>0.94332180314653835</v>
+      </c>
+      <c r="W3">
+        <v>0.61702599025741589</v>
+      </c>
+      <c r="X3">
         <v>62</v>
       </c>
+      <c r="Y3">
+        <v>69.171052631578945</v>
+      </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="D4">
         <v>12.1625</v>
       </c>
-      <c r="D4">
-        <v>0.5738068937071275</v>
-      </c>
       <c r="E4">
+        <v>0.57380689370712745</v>
+      </c>
+      <c r="F4">
         <v>14.1875</v>
       </c>
-      <c r="F4">
-        <v>0.5974878183176412</v>
-      </c>
       <c r="G4">
-        <v>2.025</v>
+        <v>0.59748781831764119</v>
       </c>
       <c r="H4">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="I4">
         <v>0.1135248773651016</v>
       </c>
-      <c r="I4">
-        <v>0.02285394666213483</v>
-      </c>
       <c r="J4">
-        <v>0.8283996887395584</v>
+        <v>2.285394666213483E-2</v>
       </c>
       <c r="K4">
-        <v>0.3601928983900611</v>
+        <v>0.82839968873955838</v>
       </c>
       <c r="L4">
+        <v>0.36019289839006108</v>
+      </c>
+      <c r="M4">
         <v>80</v>
       </c>
-      <c r="M4">
-        <v>17.15555555555556</v>
-      </c>
       <c r="N4">
-        <v>0.6805503961688807</v>
+        <v>69.848837209302332</v>
       </c>
       <c r="O4">
-        <v>19.6</v>
+        <v>17.155555555555559</v>
       </c>
       <c r="P4">
-        <v>0.7672770734003416</v>
+        <v>0.68055039616888069</v>
       </c>
       <c r="Q4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0.76727707340034157</v>
+      </c>
+      <c r="S4">
         <v>2.444444444444446</v>
       </c>
-      <c r="R4">
-        <v>0.1903114186851212</v>
-      </c>
       <c r="T4">
+        <v>0.19031141868512119</v>
+      </c>
+      <c r="V4">
         <v>1.025603699823384</v>
       </c>
-      <c r="U4">
-        <v>0.4189968136698011</v>
-      </c>
-      <c r="V4">
+      <c r="W4">
+        <v>0.41899681366980113</v>
+      </c>
+      <c r="X4">
         <v>90</v>
       </c>
+      <c r="Y4">
+        <v>72.432692307692307</v>
+      </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5">
-        <v>8.467213114754099</v>
+        <v>71.942652329749109</v>
       </c>
       <c r="D5">
-        <v>0.3570917062688789</v>
+        <v>8.4672131147540988</v>
       </c>
       <c r="E5">
-        <v>12.09016393442623</v>
+        <v>0.35709170626887887</v>
       </c>
       <c r="F5">
-        <v>0.4473353793918954</v>
+        <v>12.090163934426229</v>
       </c>
       <c r="G5">
+        <v>0.44733537939189538</v>
+      </c>
+      <c r="H5">
         <v>3.622950819672131</v>
       </c>
-      <c r="H5">
-        <v>0.1682527598020556</v>
-      </c>
       <c r="I5">
-        <v>0.01657304314922326</v>
+        <v>0.16825275980205559</v>
       </c>
       <c r="J5">
-        <v>0.5723839867970716</v>
+        <v>1.6573043149223261E-2</v>
       </c>
       <c r="K5">
-        <v>0.3502235469448585</v>
+        <v>0.57238398679707159</v>
       </c>
       <c r="L5">
+        <v>0.35022354694485852</v>
+      </c>
+      <c r="M5">
         <v>122</v>
       </c>
-      <c r="M5">
+      <c r="N5">
+        <v>70.8515625</v>
+      </c>
+      <c r="O5">
         <v>12.98837209302326</v>
       </c>
-      <c r="N5">
-        <v>0.5837503603309038</v>
-      </c>
-      <c r="O5">
-        <v>16.66279069767442</v>
-      </c>
       <c r="P5">
-        <v>0.688703149956194</v>
+        <v>0.58375036033090377</v>
       </c>
       <c r="Q5">
+        <v>16.662790697674421</v>
+      </c>
+      <c r="R5">
+        <v>0.68870314995619397</v>
+      </c>
+      <c r="S5">
         <v>3.67441860465116</v>
       </c>
-      <c r="R5">
-        <v>0.2159945317840054</v>
-      </c>
-      <c r="S5">
-        <v>0.03037152493102834</v>
-      </c>
       <c r="T5">
-        <v>0.9028158793165103</v>
+        <v>0.21599453178400541</v>
       </c>
       <c r="U5">
-        <v>0.4424288949386546</v>
+        <v>3.0371524931028342E-2</v>
       </c>
       <c r="V5">
+        <v>0.90281587931651031</v>
+      </c>
+      <c r="W5">
+        <v>0.44242889493865462</v>
+      </c>
+      <c r="X5">
         <v>86</v>
       </c>
+      <c r="Y5">
+        <v>75.065934065934073</v>
+      </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6">
+        <v>73.690909090909088</v>
+      </c>
+      <c r="D6">
         <v>12.65909090909091</v>
       </c>
-      <c r="D6">
-        <v>0.5532950512141868</v>
-      </c>
       <c r="E6">
+        <v>0.55329505121418676</v>
+      </c>
+      <c r="F6">
         <v>15.07954545454546</v>
       </c>
-      <c r="F6">
-        <v>0.5989414187727352</v>
-      </c>
       <c r="G6">
-        <v>2.420454545454547</v>
+        <v>0.59894141877273521</v>
       </c>
       <c r="H6">
-        <v>0.1395806028833552</v>
+        <v>2.4204545454545472</v>
       </c>
       <c r="I6">
-        <v>0.03027141051974356</v>
+        <v>0.13958060288335519</v>
       </c>
       <c r="J6">
-        <v>0.8153933019222114</v>
+        <v>3.0271410519743559E-2</v>
       </c>
       <c r="K6">
+        <v>0.81539330192221138</v>
+      </c>
+      <c r="L6">
         <v>0.4324004076867678</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>88</v>
       </c>
-      <c r="M6">
-        <v>18.42477876106195</v>
-      </c>
       <c r="N6">
-        <v>0.5386170234948955</v>
+        <v>75.225806451612897</v>
       </c>
       <c r="O6">
-        <v>19.35398230088495</v>
+        <v>18.424778761061951</v>
       </c>
       <c r="P6">
-        <v>0.6576545731672686</v>
+        <v>0.53861702349489549</v>
       </c>
       <c r="Q6">
-        <v>0.929203539823007</v>
+        <v>19.353982300884951</v>
       </c>
       <c r="R6">
-        <v>0.080275229357798</v>
+        <v>0.65765457316726861</v>
+      </c>
+      <c r="S6">
+        <v>0.92920353982300696</v>
       </c>
       <c r="T6">
-        <v>0.8500693122365511</v>
-      </c>
-      <c r="U6">
-        <v>0.3660093360776047</v>
+        <v>8.0275229357798003E-2</v>
       </c>
       <c r="V6">
+        <v>0.85006931223655113</v>
+      </c>
+      <c r="W6">
+        <v>0.36600933607760472</v>
+      </c>
+      <c r="X6">
         <v>113</v>
       </c>
+      <c r="Y6">
+        <v>74.9296875</v>
+      </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7">
-        <v>8.38036809815951</v>
+        <v>67.096219931271477</v>
       </c>
       <c r="D7">
-        <v>0.337758469669902</v>
+        <v>8.3803680981595097</v>
       </c>
       <c r="E7">
-        <v>13.14110429447853</v>
+        <v>0.33775846966990197</v>
       </c>
       <c r="F7">
-        <v>0.4233112369027712</v>
+        <v>13.141104294478531</v>
       </c>
       <c r="G7">
-        <v>4.760736196319018</v>
+        <v>0.42331123690277123</v>
       </c>
       <c r="H7">
-        <v>0.2202043132803632</v>
+        <v>4.7607361963190176</v>
       </c>
       <c r="I7">
-        <v>0.02606069692203975</v>
+        <v>0.22020431328036319</v>
       </c>
       <c r="J7">
-        <v>0.5415470313111393</v>
+        <v>2.6060696922039751E-2</v>
       </c>
       <c r="K7">
-        <v>0.3619644739167225</v>
+        <v>0.54154703131113935</v>
       </c>
       <c r="L7">
+        <v>0.36196447391672248</v>
+      </c>
+      <c r="M7">
         <v>163</v>
       </c>
-      <c r="M7">
-        <v>13.71604938271605</v>
-      </c>
       <c r="N7">
-        <v>0.6216849287113214</v>
+        <v>69.017647058823528</v>
       </c>
       <c r="O7">
-        <v>17.59259259259259</v>
+        <v>13.716049382716051</v>
       </c>
       <c r="P7">
-        <v>0.7618969539576407</v>
+        <v>0.62168492871132142</v>
       </c>
       <c r="Q7">
-        <v>3.876543209876543</v>
+        <v>17.592592592592592</v>
       </c>
       <c r="R7">
-        <v>0.2380591357088704</v>
+        <v>0.76189695395764068</v>
       </c>
       <c r="S7">
-        <v>0.04300290687862524</v>
+        <v>3.8765432098765431</v>
       </c>
       <c r="T7">
-        <v>0.9833509643238939</v>
+        <v>0.23805913570887041</v>
       </c>
       <c r="U7">
-        <v>0.5481119996978467</v>
+        <v>4.3002906878625242E-2</v>
       </c>
       <c r="V7">
+        <v>0.98335096432389391</v>
+      </c>
+      <c r="W7">
+        <v>0.54811199969784674</v>
+      </c>
+      <c r="X7">
         <v>81</v>
       </c>
+      <c r="Y7">
+        <v>65.086956521739125</v>
+      </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8">
+        <v>72.291390728476827</v>
+      </c>
+      <c r="D8">
         <v>13.46153846153846</v>
       </c>
-      <c r="D8">
-        <v>0.8444037846192365</v>
-      </c>
       <c r="E8">
+        <v>0.84440378461923649</v>
+      </c>
+      <c r="F8">
         <v>15.01923076923077</v>
       </c>
-      <c r="F8">
-        <v>0.8832659062239271</v>
-      </c>
       <c r="G8">
-        <v>1.557692307692308</v>
+        <v>0.88326590622392709</v>
       </c>
       <c r="H8">
-        <v>0.09418604651162794</v>
+        <v>1.5576923076923079</v>
       </c>
       <c r="I8">
-        <v>0.05372298577769118</v>
+        <v>9.4186046511627944E-2</v>
       </c>
       <c r="J8">
+        <v>5.3722985777691183E-2</v>
+      </c>
+      <c r="K8">
         <v>1.221955978166507</v>
       </c>
-      <c r="K8">
-        <v>0.5391277391388291</v>
-      </c>
       <c r="L8">
+        <v>0.53912773913882905</v>
+      </c>
+      <c r="M8">
         <v>52</v>
       </c>
-      <c r="M8">
-        <v>18.19090909090909</v>
-      </c>
       <c r="N8">
-        <v>0.6482793617466404</v>
+        <v>71.309090909090912</v>
       </c>
       <c r="O8">
-        <v>20.03636363636364</v>
+        <v>18.190909090909091</v>
       </c>
       <c r="P8">
-        <v>0.6712153060758306</v>
+        <v>0.64827936174664036</v>
       </c>
       <c r="Q8">
-        <v>1.845454545454544</v>
+        <v>20.036363636363639</v>
       </c>
       <c r="R8">
+        <v>0.67121530607583058</v>
+      </c>
+      <c r="S8">
+        <v>1.8454545454545439</v>
+      </c>
+      <c r="T8">
         <v>0.1562740569668975</v>
       </c>
-      <c r="T8">
-        <v>0.9331645717541479</v>
-      </c>
-      <c r="U8">
-        <v>0.4667754206794948</v>
-      </c>
       <c r="V8">
+        <v>0.93316457175414791</v>
+      </c>
+      <c r="W8">
+        <v>0.46677542067949479</v>
+      </c>
+      <c r="X8">
         <v>110</v>
       </c>
+      <c r="Y8">
+        <v>75.61666666666666</v>
+      </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>9.341935483870968</v>
+        <v>72.822622107969153</v>
       </c>
       <c r="D9">
-        <v>0.3613546534383871</v>
+        <v>9.3419354838709676</v>
       </c>
       <c r="E9">
-        <v>14.69677419354839</v>
+        <v>0.36135465343838707</v>
       </c>
       <c r="F9">
-        <v>0.4553249799113191</v>
+        <v>14.696774193548389</v>
       </c>
       <c r="G9">
-        <v>5.35483870967742</v>
+        <v>0.45532497991131909</v>
       </c>
       <c r="H9">
-        <v>0.259212991880075</v>
+        <v>5.3548387096774199</v>
       </c>
       <c r="I9">
-        <v>0.01840167632098874</v>
+        <v>0.25921299188007502</v>
       </c>
       <c r="J9">
-        <v>0.5812899645554016</v>
+        <v>1.8401676320988741E-2</v>
       </c>
       <c r="K9">
-        <v>0.3698686839386575</v>
+        <v>0.58128996455540161</v>
       </c>
       <c r="L9">
+        <v>0.36986868393865752</v>
+      </c>
+      <c r="M9">
         <v>155</v>
       </c>
-      <c r="M9">
+      <c r="N9">
+        <v>72.460122699386503</v>
+      </c>
+      <c r="O9">
         <v>15.06410256410256</v>
       </c>
-      <c r="N9">
-        <v>0.6585435204259115</v>
-      </c>
-      <c r="O9">
-        <v>20.2948717948718</v>
-      </c>
       <c r="P9">
-        <v>0.6093698875011779</v>
+        <v>0.65854352042591147</v>
       </c>
       <c r="Q9">
-        <v>5.230769230769232</v>
+        <v>20.294871794871799</v>
       </c>
       <c r="R9">
-        <v>0.3502145922746782</v>
+        <v>0.60936988750117793</v>
+      </c>
+      <c r="S9">
+        <v>5.2307692307692317</v>
       </c>
       <c r="T9">
-        <v>0.897224179393395</v>
-      </c>
-      <c r="U9">
+        <v>0.35021459227467822</v>
+      </c>
+      <c r="V9">
+        <v>0.89722417939339505</v>
+      </c>
+      <c r="W9">
         <v>0.4913243592729864</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>78</v>
       </c>
+      <c r="Y9">
+        <v>75.329545454545453</v>
+      </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10">
+        <v>77.84375</v>
+      </c>
+      <c r="D10">
         <v>11.97674418604651</v>
       </c>
-      <c r="D10">
-        <v>0.8113865551343201</v>
-      </c>
       <c r="E10">
-        <v>12.81395348837209</v>
+        <v>0.81138655513432012</v>
       </c>
       <c r="F10">
-        <v>0.9749099478267346</v>
+        <v>12.813953488372089</v>
       </c>
       <c r="G10">
-        <v>0.8372093023255811</v>
+        <v>0.97490994782673457</v>
       </c>
       <c r="H10">
-        <v>0.04645161290322579</v>
+        <v>0.83720930232558111</v>
       </c>
       <c r="I10">
-        <v>0.03889853635251428</v>
+        <v>4.6451612903225789E-2</v>
       </c>
       <c r="J10">
-        <v>1.268383833161029</v>
+        <v>3.8898536352514279E-2</v>
       </c>
       <c r="K10">
-        <v>0.690009575549571</v>
+        <v>1.2683838331610291</v>
       </c>
       <c r="L10">
+        <v>0.69000957554957099</v>
+      </c>
+      <c r="M10">
         <v>43</v>
       </c>
-      <c r="M10">
-        <v>17.36842105263158</v>
-      </c>
       <c r="N10">
-        <v>0.6797424964615975</v>
+        <v>83.543478260869563</v>
       </c>
       <c r="O10">
-        <v>17.2421052631579</v>
+        <v>17.368421052631579</v>
       </c>
       <c r="P10">
-        <v>0.687386890131191</v>
+        <v>0.67974249646159746</v>
       </c>
       <c r="Q10">
+        <v>17.242105263157899</v>
+      </c>
+      <c r="R10">
+        <v>0.68738689013119103</v>
+      </c>
+      <c r="S10">
         <v>-0.1263157894736828</v>
       </c>
-      <c r="R10">
-        <v>-0.009999999999999891</v>
-      </c>
-      <c r="S10">
-        <v>0.03449851527697276</v>
-      </c>
       <c r="T10">
-        <v>0.9667215722327059</v>
+        <v>-9.9999999999998909E-3</v>
       </c>
       <c r="U10">
-        <v>0.3179025977388099</v>
+        <v>3.4498515276972758E-2</v>
       </c>
       <c r="V10">
+        <v>0.96672157223270594</v>
+      </c>
+      <c r="W10">
+        <v>0.31790259773880991</v>
+      </c>
+      <c r="X10">
         <v>95</v>
       </c>
+      <c r="Y10">
+        <v>75.407079646017692</v>
+      </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11">
-        <v>9.790419161676647</v>
+        <v>73.650000000000006</v>
       </c>
       <c r="D11">
-        <v>0.3659081535133401</v>
+        <v>9.7904191616766472</v>
       </c>
       <c r="E11">
-        <v>14.10778443113773</v>
+        <v>0.36590815351334011</v>
       </c>
       <c r="F11">
-        <v>0.4384840137280439</v>
+        <v>14.107784431137731</v>
       </c>
       <c r="G11">
+        <v>0.43848401372804391</v>
+      </c>
+      <c r="H11">
         <v>4.317365269461078</v>
       </c>
-      <c r="H11">
-        <v>0.2136296296296296</v>
-      </c>
       <c r="I11">
-        <v>0.0168850133911933</v>
+        <v>0.21362962962962961</v>
       </c>
       <c r="J11">
-        <v>0.5711015733672929</v>
+        <v>1.6885013391193301E-2</v>
       </c>
       <c r="K11">
-        <v>0.318613100477558</v>
+        <v>0.57110157336729295</v>
       </c>
       <c r="L11">
+        <v>0.31861310047755798</v>
+      </c>
+      <c r="M11">
         <v>167</v>
       </c>
-      <c r="M11">
-        <v>14.45977011494253</v>
-      </c>
       <c r="N11">
-        <v>0.5754499413888345</v>
+        <v>74.032085561497325</v>
       </c>
       <c r="O11">
-        <v>18.70114942528735</v>
+        <v>14.459770114942531</v>
       </c>
       <c r="P11">
-        <v>0.6580805569134573</v>
+        <v>0.57544994138883454</v>
       </c>
       <c r="Q11">
-        <v>4.241379310344826</v>
+        <v>18.701149425287351</v>
       </c>
       <c r="R11">
+        <v>0.65808055691345735</v>
+      </c>
+      <c r="S11">
+        <v>4.2413793103448256</v>
+      </c>
+      <c r="T11">
         <v>0.2729289940828401</v>
       </c>
-      <c r="S11">
-        <v>0.03362558601135256</v>
-      </c>
-      <c r="T11">
-        <v>0.8741925728533383</v>
-      </c>
       <c r="U11">
-        <v>0.46731315739378</v>
+        <v>3.3625586011352557E-2</v>
       </c>
       <c r="V11">
+        <v>0.87419257285333829</v>
+      </c>
+      <c r="W11">
+        <v>0.46731315739377999</v>
+      </c>
+      <c r="X11">
         <v>87</v>
       </c>
+      <c r="Y11">
+        <v>73.434343434343432</v>
+      </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12">
+        <v>80.904382470119515</v>
+      </c>
+      <c r="D12">
         <v>12.33333333333333</v>
       </c>
-      <c r="D12">
-        <v>0.7072544488881022</v>
-      </c>
       <c r="E12">
+        <v>0.70725444888810218</v>
+      </c>
+      <c r="F12">
         <v>14.89473684210526</v>
       </c>
-      <c r="F12">
-        <v>0.8012694386798697</v>
-      </c>
       <c r="G12">
-        <v>2.56140350877193</v>
+        <v>0.80126943867986966</v>
       </c>
       <c r="H12">
-        <v>0.1449851042701092</v>
+        <v>2.5614035087719298</v>
       </c>
       <c r="I12">
-        <v>0.02304780461542826</v>
+        <v>0.14498510427010919</v>
       </c>
       <c r="J12">
-        <v>0.6914341384628476</v>
+        <v>2.3047804615428259E-2</v>
       </c>
       <c r="K12">
+        <v>0.69143413846284763</v>
+      </c>
+      <c r="L12">
         <v>1.068757020484248</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>57</v>
       </c>
-      <c r="M12">
-        <v>14.76576576576577</v>
-      </c>
       <c r="N12">
+        <v>82.072463768115938</v>
+      </c>
+      <c r="O12">
+        <v>14.765765765765771</v>
+      </c>
+      <c r="P12">
         <v>0.5200256647977225</v>
       </c>
-      <c r="O12">
-        <v>17.96396396396396</v>
-      </c>
-      <c r="P12">
-        <v>0.6985333796916776</v>
-      </c>
       <c r="Q12">
-        <v>3.198198198198197</v>
+        <v>17.963963963963959</v>
       </c>
       <c r="R12">
-        <v>0.2099349497338852</v>
+        <v>0.69853337969167761</v>
       </c>
       <c r="S12">
-        <v>0.01909700426514009</v>
+        <v>3.1981981981981971</v>
       </c>
       <c r="T12">
-        <v>0.572910127954203</v>
+        <v>0.20993494973388521</v>
       </c>
       <c r="U12">
-        <v>0.8708476184682317</v>
+        <v>1.9097004265140091E-2</v>
       </c>
       <c r="V12">
+        <v>0.57291012795420304</v>
+      </c>
+      <c r="W12">
+        <v>0.87084761846823167</v>
+      </c>
+      <c r="X12">
         <v>111</v>
       </c>
+      <c r="Y12">
+        <v>79.961290322580652</v>
+      </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13">
-        <v>9.376744186046512</v>
+        <v>75.842931937172779</v>
       </c>
       <c r="D13">
+        <v>9.3767441860465119</v>
+      </c>
+      <c r="E13">
         <v>0.2736919344088321</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>13.64651162790698</v>
       </c>
-      <c r="F13">
-        <v>0.3863891347290506</v>
-      </c>
       <c r="G13">
-        <v>4.269767441860465</v>
+        <v>0.38638913472905062</v>
       </c>
       <c r="H13">
-        <v>0.2070365358592693</v>
+        <v>4.2697674418604654</v>
       </c>
       <c r="I13">
-        <v>0.0103739092627643</v>
+        <v>0.20703653585926929</v>
       </c>
       <c r="J13">
-        <v>0.3112172778829289</v>
+        <v>1.0373909262764301E-2</v>
       </c>
       <c r="K13">
-        <v>0.473501677290707</v>
+        <v>0.31121727788292891</v>
       </c>
       <c r="L13">
+        <v>0.47350167729070702</v>
+      </c>
+      <c r="M13">
         <v>215</v>
       </c>
-      <c r="M13">
-        <v>12.24691358024691</v>
-      </c>
       <c r="N13">
-        <v>0.5413548573186054</v>
+        <v>75.385245901639351</v>
       </c>
       <c r="O13">
-        <v>15.75308641975309</v>
+        <v>12.246913580246909</v>
       </c>
       <c r="P13">
-        <v>0.8201796822477849</v>
+        <v>0.54135485731860544</v>
       </c>
       <c r="Q13">
-        <v>3.506172839506174</v>
+        <v>15.753086419753091</v>
       </c>
       <c r="R13">
+        <v>0.82017968224778492</v>
+      </c>
+      <c r="S13">
+        <v>3.5061728395061742</v>
+      </c>
+      <c r="T13">
         <v>0.1974965229485397</v>
       </c>
-      <c r="S13">
-        <v>0.02474924627020214</v>
-      </c>
-      <c r="T13">
-        <v>0.7424773881060645</v>
-      </c>
       <c r="U13">
-        <v>0.9827307834369111</v>
+        <v>2.4749246270202141E-2</v>
       </c>
       <c r="V13">
+        <v>0.74247738810606445</v>
+      </c>
+      <c r="W13">
+        <v>0.98273078343691112</v>
+      </c>
+      <c r="X13">
         <v>81</v>
+      </c>
+      <c r="Y13">
+        <v>76.551724137931032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>